<commit_message>
Add bank sentral annotation system
</commit_message>
<xml_diff>
--- a/data/Press_Release.xlsx
+++ b/data/Press_Release.xlsx
@@ -1601,7 +1601,7 @@
     <t>BI-Rate Naik 25 bps Menjadi 6,25%: Memperkuat Stabilitas dan Menjaga Pertumbuhan dari Dampak Rambatan Global</t>
   </si>
   <si>
-    <t>apat Dewan Gubernur (RDG) Bank Indonesia pada 23-24 April 2024 memutuskan untuk menaikkan BI-Rate sebesar 25 bps menjadi 6,25%, suku bunga Deposit Facility sebesar 25 bps menjadi 5,50%, dan suku bunga Lending Facility sebesar 25 bps menjadi 7,00%. Kenaikan suku bunga ini untuk memperkuat stabilitas nilai tukar Rupiah dari dampak memburuknya risiko global serta sebagai langkah pre-emptive dan forward looking untuk memastikan inflasi tetap dalam sasaran 2,5±1% pada 2024 dan 2025 sejalan dengan stance kebijakan moneter yang pro-stability. Sementara itu, kebijakan makroprudensial dan sistem pembayaran tetap pro-growth untuk mendukung pertumbuhan ekonomi yang berkelanjutan. Kebijakan makroprudensial longgar terus ditempuh untuk mendorong kredit/pembiayaan perbankan kepada dunia usaha dan rumah tangga. Kebijakan sistem pembayaran diarahkan untuk memperkuat keandalan infrastruktur dan struktur industri sistem pembayaran, serta memperluas akseptasi digitalisasi sistem pembayaran.
+    <t>Rapat Dewan Gubernur (RDG) Bank Indonesia pada 23-24 April 2024 memutuskan untuk menaikkan BI-Rate sebesar 25 bps menjadi 6,25%, suku bunga Deposit Facility sebesar 25 bps menjadi 5,50%, dan suku bunga Lending Facility sebesar 25 bps menjadi 7,00%. Kenaikan suku bunga ini untuk memperkuat stabilitas nilai tukar Rupiah dari dampak memburuknya risiko global serta sebagai langkah pre-emptive dan forward looking untuk memastikan inflasi tetap dalam sasaran 2,5±1% pada 2024 dan 2025 sejalan dengan stance kebijakan moneter yang pro-stability. Sementara itu, kebijakan makroprudensial dan sistem pembayaran tetap pro-growth untuk mendukung pertumbuhan ekonomi yang berkelanjutan. Kebijakan makroprudensial longgar terus ditempuh untuk mendorong kredit/pembiayaan perbankan kepada dunia usaha dan rumah tangga. Kebijakan sistem pembayaran diarahkan untuk memperkuat keandalan infrastruktur dan struktur industri sistem pembayaran, serta memperluas akseptasi digitalisasi sistem pembayaran.
 Untuk menjaga stabilitas dan mendukung pertumbuhan ekonomi yang berkelanjutan di tengah peningkatan ketidakpastian pasar keuangan global, Bank Indonesia terus memperkuat bauran kebijakan moneter, makroprudensial, dan sistem pembayaran sebagai berikut:
 Kenaikan struktur suku bunga di pasar uang Rupiah sejalan dengan kenaikan BI-Rate serta meningkatnya yield US Treasury dan premi risiko global untuk menjaga daya tarik imbal hasil dan aliran masuk portfolio asing ke aset keuangan domestik guna mendukung stabilitas nilai tukar Rupiah;
 Peningkatan stabilisasi nilai tukar Rupiah melalui intervensi di pasar valas pada transaksi spot, Domestic Non-Deliverable Forward (DNDF), dan Surat Berharga Negara (SBN) di pasar sekunder;
@@ -1611,7 +1611,7 @@
 Memperkuat Kebijakan Insentif Likuiditas Makroprudensial (KLM) untuk mendorong pertumbuhan kredit/pembiayaan melalui perluasan cakupan sektor prioritas, yakni sektor penunjang hilirisasi, konstruksi dan real estate produktif, ekonomi kreatif, otomotif, perdagangan, Listrik-Gas-Air Bersih (LGA), dan jasa sosial; serta penyesuaian besaran insentif untuk setiap sektor yang berlaku mulai 1 Juni 2024 (Lampiran 1);
 Mempertahankan: (a) Rasio Countercyclical Capital Buffer (CCyB) sebesar 0%; (b) Rasio Intermediasi Makroprudensial (RIM) pada kisaran 84-94%; (c) Rasio Penyangga Likuiditas Makroprudensial (PLM) sebesar 5% dengan fleksibilitas repo sebesar 5%, dan rasio PLM Syariah sebesar 3,5% dengan fleksibilitas repo sebesar 3,5%;
 Pendalaman kebijakan transparansi Suku Bunga Dasar Kredit (SBDK) dengan pendalaman suku bunga kredit berdasarkan sektor ekonomi (Lampiran 2);
-Penguatan literasi digital dan manajemen risiko penyelenggara dan masyarakat pengguna sistem pembayaran, termasuk berbagai inovasi yang mendukung inisiatif tersebut, guna memperkuat stabilitas sistem pembayaran dalam rangka mendukung pertumbuhan ekonomi yang berkelanjutan.
+Penguatan literasi digital dan manajemen risiko penyelenggara dan masyarakat pengguna sistem pembayaran, termasuk berbagai inovasi yang mendukung inisiatif tersebut, guna memperkuat stabilitas sistem pembayaran dalam rangka mendukung pertumbuhan ekonomi yang berkelanjutan. 
 ​Bank Indonesia terus memperkuat koordinasi kebijakan dengan Pemerintah untuk memitigasi dampak rambatan memburuknya risiko global. Untuk pengendalian inflasi, koordinasi kebijakan dengan Pemerintah (Pusat dan Daerah) melalui program Gerakan Nasional Pengendalian Inflasi Pangan (GNPIP) di berbagai daerah dalam Tim Pengendalian Inflasi Pusat dan Daerah (TPIP dan TPID). Koordinasi kebijakan moneter dan fiskal diperkuat untuk menjaga stabilitas makroekonomi dan momentum pertumbuhan ekonomi.  Bank Indonesia memperkuat sinergi kebijakan dengan Komite Stabilitas Sistem Keuangan (KSSK) untuk menjaga stabilitas sistem keuangan dan mendorong kredit/pembiayaan kepada dunia usaha. 
 Dinamika ekonomi keuangan global berubah cepat dengan risiko dan ketidakpastian meningkat karena perubahan arah kebijakan moneter AS dan memburuknya ketegangan geopolitik di Timur Tengah. Tetap tingginya inflasi dan kuatnya pertumbuhan ekonomi Amerika Serikat (AS) mendorong spekulasi penurunan Fed Funds Rate (FFR) yang lebih kecil dan lebih lama dari prakiraan (high for longer) sejalan pula dengan pernyataan para pejabat Federal Reserve System. Perkembangan ini dan besarnya kebutuhan utang AS mengakibatkan terus meningkatnya yield  US Treasury dan penguatan dolar AS semakin tinggi secara global. Semakin kuatnya dolar AS juga didorong oleh melemahnya sejumlah mata uang dunia seperti Yen Jepang dan Yuan Tiongkok. Ketidakpastian pasar keuangan global semakin buruk akibat eskalasi ketegangan geopolitik di Timur Tengah. Akibatnya, investor global memindahkan portfolionya ke aset yang lebih aman khususnya mata uang dolar AS dan emas, sehingga menyebabkan pelarian modal keluar dan pelemahan nilai tukar di negara berkembang semakin besar. Ke depan, risiko terkait arah penurunan FFR dan dinamika ketegangan geopolitik global akan terus dicermati karena dapat mendorong berlanjutnya ketidakpastian pasar keuangan global, meningkatnya tekanan inflasi, dan menurunnya prospek pertumbuhan ekonomi dunia. Kondisi ini memerlukan respons kebijakan yang kuat untuk memitigasi dampak negatif dari rambatan ketidakpastian global tersebut terhadap perekonomian di negara-negara berkembang,​ termasuk di Indonesia. 
 ​Ekonomi Indonesia tetap berdaya tahan di tengah meningkatnya ketidakpastian global. Pertumbuhan ekonomi di triwulan I dan II tahun 2024 diperkirakan akan lebih tinggi dari triwulan IV tahun 2023 didukung permintaan domestik yang tetap kuat dari konsumsi rumah tangga sejalan dengan Ramadan dan Idulf​itri 1445H. Investasi bangunan lebih tinggi dari prakiraan, ditopang oleh berlanjutnya Proyek Strategis Nasional (PSN) di sejumlah daerah dan berkembangnya properti swasta sebagai dampak positif dari insentif Pemerintah. Meskipun demikian, konsumsi rumah tangga dan investasi nonbangunan perlu terus didorong untuk mendukung berlanjutnya pemulihan ekonomi nasional. Sementara itu, kinerja ekspor barang belum kuat dipengaruhi oleh penurunan ekspor komoditas sejalan dengan harga komoditas yang turun dan permintaan dari mitra dagang utama, seperti Tiongkok, yang masih lemah. Berdasarkan Lapangan Usaha (LU), sektor Industri Pengolahan, Informasi dan Komunikasi, Perdagangan Besar dan Eceran, serta Konstruksi diprakirakan tumbuh kuat. Secara spasial, pertumbuhan ekonomi di seluruh wilayah tetap baik, didukung oleh permintaan domestik, terutama konsumsi rumah tangga. Dengan berbagai perkembangan tersebut, pertumbuhan ekonomi 2024 diprakirakan berada dalam kisaran 4,7-5,5%. Ke depan, Bank Indonesia akan terus memperkuat sinergi kebijakan dengan Pemerintah, termasuk melalui stimulus fiskal Pemerintah dengan stimulus makroprudensial Bank Indonesia, guna mendukung pertumbuhan ekonomi berkelanjutan, khususnya dari sisi permintaan domestik. 
@@ -2451,7 +2451,7 @@
       <c r="D17" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="E17" s="4" t="s">
+      <c r="E17" s="5" t="s">
         <v>50</v>
       </c>
     </row>

</xml_diff>